<commit_message>
Se sube protocolo de adquisición actualizado
</commit_message>
<xml_diff>
--- a/_documentación/Protocolo Adquisición/Planilla para registro de datos.xlsx
+++ b/_documentación/Protocolo Adquisición/Planilla para registro de datos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reposBCICompetition\BCIC-Personal\_documentación\Protocolo Adquisición\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE0C521-954F-403D-92EF-542F56598F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BF2465D-4A71-4BBF-8748-EBFEFAE1D74C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Datos de Sesión" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Datos del
 voluntario</t>
@@ -96,12 +95,15 @@
   </si>
   <si>
     <t>Nombre de archivo codificado</t>
+  </si>
+  <si>
+    <t>Identificador de voluntario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,7 +425,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -431,64 +433,67 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,171 +811,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664AA71B-4F03-4CDC-ABB7-34DF2DF5A627}">
-  <dimension ref="C2:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:E22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="33.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="15" t="s">
+    <row r="2" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-    </row>
-    <row r="4" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="10" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" s="14"/>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="21"/>
-      <c r="D6" s="22" t="s">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="3:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="15"/>
+      <c r="D6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="10" t="s">
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="23"/>
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="14"/>
+      <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="14"/>
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="14"/>
+      <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="14"/>
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="14"/>
+      <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="13"/>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="19"/>
+      <c r="D14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="14" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+      <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="18"/>
-      <c r="D17" s="19" t="s">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="18"/>
+      <c r="D18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="10" t="s">
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="14"/>
+      <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="14"/>
+      <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="13"/>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="19"/>
+      <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C7:C14"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="C19:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se realiza adquisición de EEG en busca de SSVEPs
</commit_message>
<xml_diff>
--- a/_documentación/Protocolo Adquisición/Planilla para registro de datos.xlsx
+++ b/_documentación/Protocolo Adquisición/Planilla para registro de datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Datos del
 voluntario</t>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Identificador de voluntario</t>
+  </si>
+  <si>
+    <t>Duración del trial</t>
+  </si>
+  <si>
+    <t>Duración de estímulos</t>
   </si>
 </sst>
 </file>
@@ -481,6 +487,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -492,9 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -812,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E22"/>
+  <dimension ref="C2:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,11 +835,11 @@
   <sheetData>
     <row r="2" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
@@ -868,7 +874,7 @@
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="23"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
@@ -891,98 +897,112 @@
     <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="14"/>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="14"/>
       <c r="D12" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="14"/>
       <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="14"/>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="14"/>
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="19"/>
-      <c r="D14" s="4" t="s">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="20"/>
+      <c r="D16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="16" t="s">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="17"/>
-      <c r="D16" s="2" t="s">
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+      <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="17"/>
-      <c r="D17" s="2" t="s">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+      <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="18"/>
-      <c r="D18" s="10" t="s">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="18"/>
+      <c r="D20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="13" t="s">
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="14"/>
-      <c r="D20" s="2" t="s">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="14"/>
+      <c r="D22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="14"/>
-      <c r="D21" s="2" t="s">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="14"/>
+      <c r="D23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="19"/>
-      <c r="D22" s="4" t="s">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="20"/>
+      <c r="D24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E24" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C7:C14"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="C7:C16"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C21:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>